<commit_message>
did the leg work for the items and powerup classes, just need to implement on the client side now. Did some tweaks with the bullet class. added in some additional dev tools into the gameManager and gameState class. put a Random object into the Utils class for system wide use, insures extra randomness lol. Made a powerup manager which spawns new powerups every so often, but need to implement a way for it to know where to spawn power ups and which ones to spawn.
</commit_message>
<xml_diff>
--- a/Data for Development.xlsx
+++ b/Data for Development.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>bullets</t>
+  </si>
+  <si>
+    <t>speed potion</t>
+  </si>
+  <si>
+    <t>PowerUp</t>
   </si>
 </sst>
 </file>
@@ -589,10 +595,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,6 +646,14 @@
         <v>11</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -648,15 +662,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="8"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -691,6 +706,14 @@
         <v>15</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
deleted an unneeded js file. made some new node classes for use in the game, such as node, gridlockednode, and powerupnode. Did a more robust job on the powerup system that is super flexible and cool. flags will be coming soon. players now check to see if they collide with any of the items in the game state, if so and they don't have an item yet, they pick them up.
</commit_message>
<xml_diff>
--- a/Data for Development.xlsx
+++ b/Data for Development.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -74,7 +74,10 @@
     <t>speed potion</t>
   </si>
   <si>
-    <t>PowerUp</t>
+    <t>PowerUp grabbed</t>
+  </si>
+  <si>
+    <t>PowerUp draw</t>
   </si>
 </sst>
 </file>
@@ -595,7 +598,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -604,6 +607,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="8"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -651,6 +655,14 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
deleted a couple older files. finished implementing power ups on server and client side, works well so far with the speed potion only. made some performance tweaks with the message sending so that only sends the client the data that it needs (this is actually super fucking important and i deserve a raise).
</commit_message>
<xml_diff>
--- a/Data for Development.xlsx
+++ b/Data for Development.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -74,10 +74,7 @@
     <t>speed potion</t>
   </si>
   <si>
-    <t>PowerUp grabbed</t>
-  </si>
-  <si>
-    <t>PowerUp draw</t>
+    <t>Item draw</t>
   </si>
 </sst>
 </file>
@@ -598,7 +595,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -655,14 +652,6 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed and streamlined the class heirarchy so that 1) all entities now have a unique entity id 2) players and ai_players are based off a single GameCharacter class which allows some functionsto overlap (really useful). Started work on two new power ups, the chill pill and the med pack. got rid of some old useless javascript files. mostly implemented client-side entity interpolation, which allows for smoother opponent movements as well as some other server based entities.
</commit_message>
<xml_diff>
--- a/Data for Development.xlsx
+++ b/Data for Development.xlsx
@@ -9,7 +9,10 @@
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
     <sheet name="Object Code" sheetId="2" r:id="rId2"/>
-    <sheet name="Image ID" sheetId="3" r:id="rId3"/>
+    <sheet name="Client Player Message" sheetId="4" r:id="rId3"/>
+    <sheet name="Other Player Message" sheetId="5" r:id="rId4"/>
+    <sheet name="Bullet Message" sheetId="6" r:id="rId5"/>
+    <sheet name="Image ID" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -75,6 +78,96 @@
   </si>
   <si>
     <t>Item draw</t>
+  </si>
+  <si>
+    <t>add wall</t>
+  </si>
+  <si>
+    <t>remove wall</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>"000"</t>
+  </si>
+  <si>
+    <t>highest snapshot</t>
+  </si>
+  <si>
+    <t>client id</t>
+  </si>
+  <si>
+    <t>image id</t>
+  </si>
+  <si>
+    <t>sprite index</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>rotation</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>team</t>
+  </si>
+  <si>
+    <t>current weapon</t>
+  </si>
+  <si>
+    <t>item(empty/imageid)</t>
+  </si>
+  <si>
+    <t>health</t>
+  </si>
+  <si>
+    <t>is_invincible</t>
+  </si>
+  <si>
+    <t>speed_boost</t>
+  </si>
+  <si>
+    <t>damage_boost</t>
+  </si>
+  <si>
+    <t>visibility</t>
+  </si>
+  <si>
+    <t>"001"</t>
+  </si>
+  <si>
+    <t>speed</t>
+  </si>
+  <si>
+    <t>damage</t>
+  </si>
+  <si>
+    <t>xRatio</t>
+  </si>
+  <si>
+    <t>yRatio</t>
+  </si>
+  <si>
+    <t>interpolating entity</t>
   </si>
 </sst>
 </file>
@@ -595,10 +688,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,6 +748,40 @@
         <v>17</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -662,6 +789,445 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>

</xml_diff>

<commit_message>
worked on flags and some basic stuff with game/player stats
</commit_message>
<xml_diff>
--- a/Data for Development.xlsx
+++ b/Data for Development.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -168,6 +168,36 @@
   </si>
   <si>
     <t>interpolating entity</t>
+  </si>
+  <si>
+    <t>M1911</t>
+  </si>
+  <si>
+    <t>Pistol</t>
+  </si>
+  <si>
+    <t>Remington 870</t>
+  </si>
+  <si>
+    <t>Sawed-Off Shotgun</t>
+  </si>
+  <si>
+    <t>SMG</t>
+  </si>
+  <si>
+    <t>Assault Rifle</t>
+  </si>
+  <si>
+    <t>Machine Gun</t>
+  </si>
+  <si>
+    <t>Smoke Grenade</t>
+  </si>
+  <si>
+    <t>Artillery</t>
+  </si>
+  <si>
+    <t>flags</t>
   </si>
 </sst>
 </file>
@@ -580,12 +610,12 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -609,15 +639,21 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="4"/>
+      <c r="A2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -625,7 +661,9 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -633,7 +671,9 @@
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -641,7 +681,9 @@
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -649,7 +691,9 @@
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -657,7 +701,9 @@
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -665,7 +711,9 @@
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -690,7 +738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1229,10 +1277,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1281,6 +1329,14 @@
         <v>16</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
worked a bit more on flags and switching different objects over to the interpolating entity style.
</commit_message>
<xml_diff>
--- a/Data for Development.xlsx
+++ b/Data for Development.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1279,7 +1279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed a bug where the server would crash when a player died without an item (null pointer, duh). adding in the NEW game score GUI, which keeps track of the current game score in a moderately nice fashion on the client side, based off of messages from the server. started to implement stats tracking; only keeping track of CTF based stuff for now, will do kills and deaths soon! Going to start work soon on a new power up called RageSerum (damage booster)! Exciting shit.
</commit_message>
<xml_diff>
--- a/Data for Development.xlsx
+++ b/Data for Development.xlsx
@@ -4,15 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
     <sheet name="Object Code" sheetId="2" r:id="rId2"/>
     <sheet name="Client Player Message" sheetId="4" r:id="rId3"/>
     <sheet name="Other Player Message" sheetId="5" r:id="rId4"/>
-    <sheet name="Bullet Message" sheetId="6" r:id="rId5"/>
-    <sheet name="Image ID" sheetId="3" r:id="rId6"/>
+    <sheet name="Image ID" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -53,9 +52,6 @@
     <t>player</t>
   </si>
   <si>
-    <t>bullet</t>
-  </si>
-  <si>
     <t>sound</t>
   </si>
   <si>
@@ -77,9 +73,6 @@
     <t>speed potion</t>
   </si>
   <si>
-    <t>Item draw</t>
-  </si>
-  <si>
     <t>add wall</t>
   </si>
   <si>
@@ -152,21 +145,6 @@
     <t>visibility</t>
   </si>
   <si>
-    <t>"001"</t>
-  </si>
-  <si>
-    <t>speed</t>
-  </si>
-  <si>
-    <t>damage</t>
-  </si>
-  <si>
-    <t>xRatio</t>
-  </si>
-  <si>
-    <t>yRatio</t>
-  </si>
-  <si>
     <t>interpolating entity</t>
   </si>
   <si>
@@ -198,6 +176,9 @@
   </si>
   <si>
     <t>flags</t>
+  </si>
+  <si>
+    <t>game status</t>
   </si>
 </sst>
 </file>
@@ -609,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,10 +621,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -652,7 +633,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -662,7 +643,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -672,7 +653,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -682,7 +663,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -692,7 +673,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -702,7 +683,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -712,7 +693,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -738,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,7 +750,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -777,24 +758,18 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
@@ -806,7 +781,7 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -814,7 +789,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -822,7 +797,7 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -851,10 +826,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -862,7 +837,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -870,7 +845,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -878,7 +853,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -886,7 +861,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -894,7 +869,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -902,7 +877,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -910,7 +885,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -918,7 +893,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -926,7 +901,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -934,7 +909,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -942,7 +917,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -950,7 +925,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -958,7 +933,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -966,7 +941,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -974,7 +949,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -982,7 +957,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -990,7 +965,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -998,7 +973,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1006,7 +981,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1014,7 +989,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1038,10 +1013,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1049,7 +1024,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1057,7 +1032,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1065,7 +1040,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1073,7 +1048,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1081,7 +1056,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1089,7 +1064,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1097,7 +1072,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1105,7 +1080,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1113,7 +1088,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1121,7 +1096,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1130,152 +1105,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1291,10 +1120,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1302,7 +1131,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1310,7 +1139,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1318,7 +1147,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1326,7 +1155,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1334,7 +1163,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
worked on player stats. worked on artillery class. worked on player progression.
</commit_message>
<xml_diff>
--- a/Data for Development.xlsx
+++ b/Data for Development.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
     <sheet name="Object Code" sheetId="2" r:id="rId2"/>
-    <sheet name="Client Player Message" sheetId="4" r:id="rId3"/>
-    <sheet name="Other Player Message" sheetId="5" r:id="rId4"/>
-    <sheet name="Image ID" sheetId="3" r:id="rId5"/>
+    <sheet name="XP Scaling" sheetId="6" r:id="rId3"/>
+    <sheet name="Client Player Message" sheetId="4" r:id="rId4"/>
+    <sheet name="Other Player Message" sheetId="5" r:id="rId5"/>
+    <sheet name="Image ID" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -179,6 +180,12 @@
   </si>
   <si>
     <t>game status</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>XP</t>
   </si>
 </sst>
 </file>
@@ -294,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -308,6 +315,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,7 +732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -812,6 +825,233 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2750</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>3550</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>3700</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>3850</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>4400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>4900</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>5000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -998,7 +1238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -1104,7 +1344,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>

</xml_diff>

<commit_message>
made a small change to the gameState class which includes the sound message code when sending sound data to clients
</commit_message>
<xml_diff>
--- a/Data for Development.xlsx
+++ b/Data for Development.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -732,7 +732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -828,7 +828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
started filling out the gamestate subclasses so CTF based stuff is only in the CTF class. Made it so when you are the first person to join the lobby you are randomly selected to be red or blue. added some new classes for particle effects which allowed me to get the explosion animation working across the server!!!
</commit_message>
<xml_diff>
--- a/Data for Development.xlsx
+++ b/Data for Development.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -186,6 +186,18 @@
   </si>
   <si>
     <t>XP</t>
+  </si>
+  <si>
+    <t>particle effect</t>
+  </si>
+  <si>
+    <t>ground mask</t>
+  </si>
+  <si>
+    <t>ammo</t>
+  </si>
+  <si>
+    <t>boom</t>
   </si>
 </sst>
 </file>
@@ -732,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,10 +790,16 @@
       <c r="A5" s="8">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1346,10 +1364,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1406,6 +1424,30 @@
         <v>50</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>